<commit_message>
models and quantization script updated
model summaries updated, quantization script updated to save the quantized model under the postqat folder as well, quantized models also available under that folder.
</commit_message>
<xml_diff>
--- a/trained_models/MLP/balance_scale/results_table.xlsx
+++ b/trained_models/MLP/balance_scale/results_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>orig-fxp-drop</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>fxppo2_accuracy_qkeras</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>orig-fxppo2-drop_qkeras</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,6 +536,12 @@
       <c r="J2" t="n">
         <v>-0.005291005291005346</v>
       </c>
+      <c r="K2" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.005291005291005235</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -568,6 +584,12 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
+      <c r="K3" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -610,6 +632,12 @@
       <c r="J4" t="n">
         <v>0</v>
       </c>
+      <c r="K4" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -652,6 +680,12 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
+      <c r="K5" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -694,6 +728,12 @@
       <c r="J6" t="n">
         <v>0.005291005291005235</v>
       </c>
+      <c r="K6" t="n">
+        <v>0.7513227513227513</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.126984126984127</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -736,6 +776,12 @@
       <c r="J7" t="n">
         <v>-0.005291005291005235</v>
       </c>
+      <c r="K7" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -778,6 +824,12 @@
       <c r="J8" t="n">
         <v>-0.01587301587301593</v>
       </c>
+      <c r="K8" t="n">
+        <v>0.7513227513227513</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.1164021164021164</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -820,6 +872,12 @@
       <c r="J9" t="n">
         <v>-0.01058201058201058</v>
       </c>
+      <c r="K9" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.01058201058201058</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -862,6 +920,12 @@
       <c r="J10" t="n">
         <v>-0.01587301587301593</v>
       </c>
+      <c r="K10" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-0.01587301587301593</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -904,6 +968,12 @@
       <c r="J11" t="n">
         <v>-0.01058201058201058</v>
       </c>
+      <c r="K11" t="n">
+        <v>0.8783068783068783</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -946,6 +1016,12 @@
       <c r="J12" t="n">
         <v>-0.005291005291005235</v>
       </c>
+      <c r="K12" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -988,6 +1064,12 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
+      <c r="K13" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1030,6 +1112,12 @@
       <c r="J14" t="n">
         <v>0</v>
       </c>
+      <c r="K14" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1072,6 +1160,12 @@
       <c r="J15" t="n">
         <v>-0.005291005291005346</v>
       </c>
+      <c r="K15" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1114,6 +1208,12 @@
       <c r="J16" t="n">
         <v>-0.02116402116402116</v>
       </c>
+      <c r="K16" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L16" t="n">
+        <v>-0.01587301587301593</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1156,6 +1256,12 @@
       <c r="J17" t="n">
         <v>0</v>
       </c>
+      <c r="K17" t="n">
+        <v>0.8835978835978836</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1198,6 +1304,12 @@
       <c r="J18" t="n">
         <v>-0.01058201058201058</v>
       </c>
+      <c r="K18" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-0.02116402116402116</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1240,6 +1352,12 @@
       <c r="J19" t="n">
         <v>-0.005291005291005346</v>
       </c>
+      <c r="K19" t="n">
+        <v>0.7936507936507936</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.09523809523809523</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1282,6 +1400,12 @@
       <c r="J20" t="n">
         <v>0</v>
       </c>
+      <c r="K20" t="n">
+        <v>0.4603174603174603</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1323,6 +1447,12 @@
       </c>
       <c r="J21" t="n">
         <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.1746031746031745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>